<commit_message>
Updated BOM .csv and .xlsx
Updated the BOM .csv and .xlsx files in the REV20220427A directory.
</commit_message>
<xml_diff>
--- a/Accessories/ExpansionBoard_Knob/REV20220427A/BOM_Encoder_Expansion_Board_Project.xlsx
+++ b/Accessories/ExpansionBoard_Knob/REV20220427A/BOM_Encoder_Expansion_Board_Project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Altium\Encoder Board\Project Outputs for Encoder_Expansion_Board_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Altium\ExpansionBoard_Knob\REV20220427A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849242AF-30B3-41FE-B4E5-A35155475224}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3536972C-99CD-4B53-9A85-6E4989E473D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="57">
   <si>
     <t>Comment</t>
   </si>
@@ -163,34 +163,49 @@
   </si>
   <si>
     <t>JP1</t>
+  </si>
+  <si>
+    <t>Digi-Key Part Number</t>
+  </si>
+  <si>
+    <t>296-30087-1-ND</t>
+  </si>
+  <si>
+    <t>Capacitor 0.1uF</t>
+  </si>
+  <si>
+    <t>1276-1012-1-ND</t>
+  </si>
+  <si>
+    <t>AE10921-ND</t>
+  </si>
+  <si>
+    <t>609-2801-ND</t>
+  </si>
+  <si>
+    <t>732-5316-ND</t>
+  </si>
+  <si>
+    <t>PEC12R-4220F-S0024-ND</t>
+  </si>
+  <si>
+    <t>311-0.0ERCT-ND</t>
+  </si>
+  <si>
+    <t>P10.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>311-100KLDCT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="4"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="8"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -303,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -311,11 +326,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,305 +644,340 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="2" max="3" width="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>4</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>0.4</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>3.27</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>29.68</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>0.81</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>6.87</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>1.59</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>14.03</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>0.13</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="4">
         <v>1.3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>0.1</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="4">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>5</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>0.5</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <v>2.65</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>2</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>0.2</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>1.64</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="4">
         <v>14.63</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G11">
-        <f>SUM(G2:G10)</f>
-        <v>8.64</v>
-      </c>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
       <c r="H11">
         <f>SUM(H2:H10)</f>
+        <v>8.64</v>
+      </c>
+      <c r="I11">
+        <f>SUM(I2:I10)</f>
         <v>71.709999999999994</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G12">
-        <f>SUM(G2:G10)</f>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="H12">
+        <f>SUM(H2:H10)</f>
         <v>8.64</v>
       </c>
-      <c r="H12">
-        <f>SUM(H2:H10)/10</f>
+      <c r="I12">
+        <f>SUM(I2:I10)/10</f>
         <v>7.1709999999999994</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a lpf .svg file and fixed the BOM
I added a low pass filter .svg file. This file doesn't belong in this repository, however I will upload it so it can be transferred to the docs.amdc.dev website at a later date. The BOM also had an error, where the sig dif part listed was incorrect.
</commit_message>
<xml_diff>
--- a/Accessories/ExpansionBoard_Knob/REV20220427A/BOM_Encoder_Expansion_Board_Project.xlsx
+++ b/Accessories/ExpansionBoard_Knob/REV20220427A/BOM_Encoder_Expansion_Board_Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Altium\ExpansionBoard_Knob\REV20220427A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12183\Documents\GitHub\AMDC-Hardware\Accessories\ExpansionBoard_Knob\REV20220427A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3536972C-99CD-4B53-9A85-6E4989E473D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A4B0B8-AD19-4A46-A503-E64654F946AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Encoder_Expansion_Board_Pro" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,23 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BOM_Encoder_Expansion_Board_Pro!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Comment</t>
   </si>
@@ -168,9 +180,6 @@
     <t>Digi-Key Part Number</t>
   </si>
   <si>
-    <t>296-30087-1-ND</t>
-  </si>
-  <si>
     <t>Capacitor 0.1uF</t>
   </si>
   <si>
@@ -196,6 +205,9 @@
   </si>
   <si>
     <t>311-100KLDCT-ND</t>
+  </si>
+  <si>
+    <t>AM26C31CNS</t>
   </si>
 </sst>
 </file>
@@ -694,10 +706,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -726,7 +738,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -755,7 +767,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>17</v>
@@ -784,7 +796,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -813,7 +825,7 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -842,7 +854,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
@@ -871,7 +883,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>25</v>
@@ -900,7 +912,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>25</v>
@@ -928,8 +940,8 @@
       <c r="A10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
-        <v>47</v>
+      <c r="B10" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>31</v>

</xml_diff>